<commit_message>
Protocoll version 2 updated (there was a bug in the byte calculation, always 4 Bytes too much)
</commit_message>
<xml_diff>
--- a/docs/YYMMDD_A042_Protokoll_PF.xlsx
+++ b/docs/YYMMDD_A042_Protokoll_PF.xlsx
@@ -273,8 +273,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1..10
-</t>
+1, 2, 3 . . .
+Ende muss noch definiert werden!</t>
         </r>
       </text>
     </comment>
@@ -309,30 +309,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>fleischp:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Feedback Instruction is always "Reply"</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B17" authorId="0" shapeId="0">
       <text>
         <r>
@@ -356,8 +332,6 @@
 0=No Feedback
 1=Feedback
 20…for User
-**************************************************
-- Max können 20 Task auf einem Kontroller arbeiten!
 </t>
         </r>
       </text>
@@ -382,7 +356,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Done
+Feedbacklevel 1 = Done
 Done FError "Feedback Level"  (Unsupportet Feedback Level)
  </t>
         </r>
@@ -434,7 +408,8 @@
           </rPr>
           <t xml:space="preserve">
 Min 0
-Max 5</t>
+Max 8
+</t>
         </r>
       </text>
     </comment>
@@ -459,7 +434,8 @@
           </rPr>
           <t xml:space="preserve">
 Min 0
-Max 30</t>
+Max 36
+</t>
         </r>
       </text>
     </comment>
@@ -757,7 +733,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="178">
   <si>
     <t xml:space="preserve">Header </t>
   </si>
@@ -1254,15 +1230,6 @@
     <t>St8_Len</t>
   </si>
   <si>
-    <t>with</t>
-  </si>
-  <si>
-    <t>eight</t>
-  </si>
-  <si>
-    <t>strings</t>
-  </si>
-  <si>
     <t>V31</t>
   </si>
   <si>
@@ -1297,6 +1264,9 @@
   </si>
   <si>
     <t>Value 36</t>
+  </si>
+  <si>
+    <t>r_A042_Dummy</t>
   </si>
 </sst>
 </file>
@@ -3177,7 +3147,7 @@
   <dimension ref="A1:H77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3269,7 +3239,7 @@
       </c>
       <c r="C7" s="12">
         <f>SUM(D7:D74)</f>
-        <v>132</v>
+        <v>64</v>
       </c>
       <c r="D7" s="4">
         <v>4</v>
@@ -3441,7 +3411,7 @@
       </c>
       <c r="C15" s="12">
         <f>LEN(C16)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D15" s="4">
         <v>4</v>
@@ -3467,11 +3437,11 @@
         <v>7</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="D16" s="13">
         <f>C15</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -3597,9 +3567,9 @@
       <c r="B21" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="12">
         <f>COUNTA(C23,C25,C27,C29,C31)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D21" s="4">
         <v>4</v>
@@ -3626,11 +3596,11 @@
       </c>
       <c r="C22" s="12">
         <f>LEN(C23)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D22" s="13">
         <f>IF(C22&gt;=1,4,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F22" s="4">
         <v>4</v>
@@ -3649,12 +3619,10 @@
       <c r="B23" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>88</v>
-      </c>
+      <c r="C23" s="11"/>
       <c r="D23" s="13">
         <f>C22</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F23" s="4">
         <v>80</v>
@@ -3675,11 +3643,11 @@
       </c>
       <c r="C24" s="12">
         <f>LEN(C25)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24" s="13">
         <f>IF(C24&gt;=1,4,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F24" s="4">
         <v>4</v>
@@ -3698,12 +3666,10 @@
       <c r="B25" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>89</v>
-      </c>
+      <c r="C25" s="11"/>
       <c r="D25" s="13">
         <f>C24</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F25" s="4">
         <v>80</v>
@@ -3724,11 +3690,11 @@
       </c>
       <c r="C26" s="12">
         <f>LEN(C27)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="13">
         <f>IF(C26&gt;=1,4,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F26" s="4">
         <v>4</v>
@@ -3747,12 +3713,10 @@
       <c r="B27" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>90</v>
-      </c>
+      <c r="C27" s="11"/>
       <c r="D27" s="13">
         <f>C26</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="4">
         <v>80</v>
@@ -3773,11 +3737,11 @@
       </c>
       <c r="C28" s="12">
         <f>LEN(C29)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D28" s="13">
         <f>IF(C28&gt;=1,4,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F28" s="4">
         <v>4</v>
@@ -3796,12 +3760,10 @@
       <c r="B29" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>91</v>
-      </c>
+      <c r="C29" s="11"/>
       <c r="D29" s="13">
         <f>C28</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F29" s="4">
         <v>80</v>
@@ -3822,11 +3784,11 @@
       </c>
       <c r="C30" s="12">
         <f>LEN(C31)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D30" s="13">
         <f>IF(C30&gt;=1,4,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F30" s="4">
         <v>4</v>
@@ -3845,12 +3807,10 @@
       <c r="B31" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>92</v>
-      </c>
+      <c r="C31" s="11"/>
       <c r="D31" s="13">
         <f>C30</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F31" s="4">
         <v>80</v>
@@ -3871,11 +3831,11 @@
       </c>
       <c r="C32" s="12">
         <f>LEN(C33)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D32" s="13">
         <f>IF(C32&gt;=1,4,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F32" s="4">
         <v>4</v>
@@ -3894,12 +3854,10 @@
       <c r="B33" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>165</v>
-      </c>
+      <c r="C33" s="11"/>
       <c r="D33" s="13">
         <f>C32</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F33" s="4">
         <v>80</v>
@@ -3920,11 +3878,11 @@
       </c>
       <c r="C34" s="12">
         <f>LEN(C35)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D34" s="13">
         <f>IF(C34&gt;=1,4,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F34" s="4">
         <v>4</v>
@@ -3943,12 +3901,10 @@
       <c r="B35" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>166</v>
-      </c>
+      <c r="C35" s="11"/>
       <c r="D35" s="13">
         <f>C34</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F35" s="4">
         <v>80</v>
@@ -3969,11 +3925,11 @@
       </c>
       <c r="C36" s="12">
         <f>LEN(C37)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D36" s="13">
         <f>IF(C36&gt;=1,4,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F36" s="4">
         <v>4</v>
@@ -3992,12 +3948,10 @@
       <c r="B37" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>167</v>
-      </c>
+      <c r="C37" s="11"/>
       <c r="D37" s="13">
         <f>C36</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F37" s="4">
         <v>80</v>
@@ -4016,9 +3970,9 @@
       <c r="B38" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="12">
         <f>COUNTA(C39:C74)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="4">
         <v>4</v>
@@ -4043,11 +3997,10 @@
       <c r="B39" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="11">
-        <v>99</v>
-      </c>
+      <c r="C39" s="11"/>
       <c r="D39" s="13">
-        <v>4</v>
+        <f>IF(C39&gt;=1,4,0)</f>
+        <v>0</v>
       </c>
       <c r="F39" s="4">
         <v>4</v>
@@ -4699,10 +4652,10 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B69" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="13">
@@ -4721,10 +4674,10 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B70" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="13">
@@ -4743,10 +4696,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B71" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="13">
@@ -4765,10 +4718,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B72" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="13">
@@ -4787,10 +4740,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B73" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="13">
@@ -4809,10 +4762,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B74" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C74" s="11"/>
       <c r="D74" s="13">
@@ -4837,7 +4790,7 @@
       <c r="C76" s="15"/>
       <c r="D76" s="16">
         <f>SUM(D6:D74)</f>
-        <v>132</v>
+        <v>64</v>
       </c>
       <c r="E76" s="17">
         <f>SUM(E6:E74)</f>

</xml_diff>

<commit_message>
small optimisation only unit corrected (ms -> s)
</commit_message>
<xml_diff>
--- a/docs/YYMMDD_A042_Protokoll_PF.xlsx
+++ b/docs/YYMMDD_A042_Protokoll_PF.xlsx
@@ -1564,9 +1564,6 @@
     <t>Info</t>
   </si>
   <si>
-    <t>Time [ms]</t>
-  </si>
-  <si>
     <t>Max RRC Data</t>
   </si>
   <si>
@@ -1589,6 +1586,9 @@
   </si>
   <si>
     <t>Performance Rechnung</t>
+  </si>
+  <si>
+    <t>Time [s]</t>
   </si>
 </sst>
 </file>
@@ -1871,12 +1871,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1899,14 +1893,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1916,15 +1904,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1977,6 +1956,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2275,36 +2275,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -2334,16 +2334,16 @@
     </row>
     <row r="5" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="A6" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2454,16 +2454,16 @@
       <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -3690,36 +3690,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -3749,16 +3749,16 @@
     </row>
     <row r="5" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="A6" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -3869,16 +3869,16 @@
       <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -5438,7 +5438,7 @@
   <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5450,24 +5450,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="52" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -5476,7 +5476,7 @@
       <c r="B4" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -5485,12 +5485,12 @@
     </row>
     <row r="5" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="A6" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -5551,12 +5551,12 @@
     </row>
     <row r="11" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -5652,7 +5652,7 @@
       <c r="B19" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="18" t="s">
         <v>166</v>
       </c>
       <c r="D19" s="10">
@@ -5713,7 +5713,7 @@
       <c r="B23" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="17" t="s">
         <v>158</v>
       </c>
       <c r="D23" s="10">
@@ -5744,7 +5744,7 @@
       <c r="B25" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="17" t="s">
         <v>159</v>
       </c>
       <c r="D25" s="10">
@@ -5775,7 +5775,7 @@
       <c r="B27" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="17" t="s">
         <v>160</v>
       </c>
       <c r="D27" s="10">
@@ -5806,7 +5806,7 @@
       <c r="B29" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="17" t="s">
         <v>161</v>
       </c>
       <c r="D29" s="10">
@@ -5837,7 +5837,7 @@
       <c r="B31" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="17" t="s">
         <v>162</v>
       </c>
       <c r="D31" s="10">
@@ -5868,7 +5868,7 @@
       <c r="B33" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="19"/>
+      <c r="C33" s="17"/>
       <c r="D33" s="10">
         <f>C32</f>
         <v>0</v>
@@ -5897,7 +5897,7 @@
       <c r="B35" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="19"/>
+      <c r="C35" s="17"/>
       <c r="D35" s="10">
         <f>C34</f>
         <v>0</v>
@@ -5926,7 +5926,7 @@
       <c r="B37" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="19"/>
+      <c r="C37" s="17"/>
       <c r="D37" s="10">
         <f>C36</f>
         <v>0</v>
@@ -6474,7 +6474,7 @@
         <v>2</v>
       </c>
       <c r="B76" s="12"/>
-      <c r="C76" s="18"/>
+      <c r="C76" s="16"/>
       <c r="D76" s="13">
         <f>SUM(D6:D74)</f>
         <v>700</v>
@@ -6498,7 +6498,7 @@
   <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:XFD6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6510,24 +6510,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="52" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -6545,12 +6545,12 @@
     </row>
     <row r="5" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="A6" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -6613,12 +6613,12 @@
       <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -6714,7 +6714,7 @@
       <c r="B19" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="19" t="s">
         <v>170</v>
       </c>
       <c r="D19" s="10">
@@ -7497,8 +7497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7518,57 +7518,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="J2" s="51" t="s">
+        <v>202</v>
+      </c>
+      <c r="K2" s="55" t="s">
+        <v>207</v>
+      </c>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="45"/>
+    </row>
+    <row r="3" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="39"/>
+      <c r="B3" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>209</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="55" t="s">
-        <v>194</v>
-      </c>
-      <c r="J2" s="58" t="s">
-        <v>203</v>
-      </c>
-      <c r="K2" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="52"/>
-    </row>
-    <row r="3" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>201</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>196</v>
@@ -7582,330 +7582,330 @@
       <c r="G3" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="56"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="49"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="54"/>
-    </row>
-    <row r="4" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="54"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="47"/>
+    </row>
+    <row r="4" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="47"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="22">
         <v>2641</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="22">
         <v>24.354835000000001</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="24">
         <v>674</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="57">
+      <c r="I5" s="29"/>
+      <c r="J5" s="50">
         <v>620</v>
       </c>
-      <c r="K5" s="38" t="s">
-        <v>202</v>
+      <c r="K5" s="54" t="s">
+        <v>201</v>
       </c>
       <c r="L5" t="s">
         <v>176</v>
       </c>
-      <c r="M5" s="22">
+      <c r="M5" s="20">
         <f>SUM(J5:J6)</f>
         <v>1320</v>
       </c>
-      <c r="N5" s="52" t="s">
+      <c r="N5" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="O5" s="52"/>
+      <c r="O5" s="45"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="41" t="s">
         <v>191</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="22">
         <v>2643</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="22">
         <v>24.446379</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="24">
         <v>754</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="30">
         <f>(C6-C5)*1000</f>
         <v>91.54399999999896</v>
       </c>
-      <c r="J6" s="57">
+      <c r="J6" s="50">
         <v>700</v>
       </c>
-      <c r="K6" s="38"/>
+      <c r="K6" s="54"/>
       <c r="L6" t="s">
         <v>179</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="20">
         <f>I6</f>
         <v>91.54399999999896</v>
       </c>
-      <c r="N6" s="52" t="s">
+      <c r="N6" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="O6" s="52"/>
+      <c r="O6" s="45"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="57"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="50"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="45"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="41" t="s">
         <v>192</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="22">
         <v>2792</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="22">
         <v>24.978383000000001</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="24">
         <v>114</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="I8" s="33"/>
-      <c r="J8" s="57">
+      <c r="I8" s="29"/>
+      <c r="J8" s="50">
         <v>60</v>
       </c>
-      <c r="K8" s="38" t="s">
-        <v>204</v>
+      <c r="K8" s="54" t="s">
+        <v>203</v>
       </c>
       <c r="L8" t="s">
         <v>176</v>
       </c>
-      <c r="M8" s="22">
+      <c r="M8" s="20">
         <f>SUM(J8:J9)</f>
         <v>121</v>
       </c>
-      <c r="N8" s="52" t="s">
+      <c r="N8" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="O8" s="52"/>
+      <c r="O8" s="45"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="41" t="s">
         <v>193</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="22">
         <v>2793</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="22">
         <v>25.035176</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="24">
         <v>115</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="I9" s="34">
+      <c r="I9" s="30">
         <f>(C9-C8)*1000</f>
         <v>56.792999999998983</v>
       </c>
-      <c r="J9" s="57">
+      <c r="J9" s="50">
         <v>61</v>
       </c>
-      <c r="K9" s="38"/>
+      <c r="K9" s="54"/>
       <c r="L9" t="s">
         <v>179</v>
       </c>
-      <c r="M9" s="22">
+      <c r="M9" s="20">
         <f>I9</f>
         <v>56.792999999998983</v>
       </c>
-      <c r="N9" s="52" t="s">
+      <c r="N9" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="O9" s="52"/>
+      <c r="O9" s="45"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="52"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="N10" s="45"/>
+      <c r="O10" s="45"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="38" t="s">
-        <v>205</v>
+      <c r="A11" s="42"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="54" t="s">
+        <v>204</v>
       </c>
       <c r="L11" t="s">
         <v>183</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="20">
         <f>M5-M8</f>
         <v>1199</v>
       </c>
-      <c r="N11" s="52" t="s">
+      <c r="N11" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="O11" s="52"/>
+      <c r="O11" s="45"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="38"/>
+      <c r="A12" s="42"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="54"/>
       <c r="L12" t="s">
         <v>184</v>
       </c>
-      <c r="M12" s="22">
+      <c r="M12" s="20">
         <f>M6-M9</f>
         <v>34.750999999999976</v>
       </c>
-      <c r="N12" s="52" t="s">
+      <c r="N12" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="O12" s="52"/>
+      <c r="O12" s="45"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="38"/>
+      <c r="A13" s="42"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="54"/>
       <c r="L13" t="s">
         <v>185</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="20">
         <f>M12/M11</f>
         <v>2.8983319432860699E-2</v>
       </c>
-      <c r="N13" s="52" t="s">
+      <c r="N13" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="O13" s="52"/>
+      <c r="O13" s="45"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="52"/>
+      <c r="A14" s="42"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="45"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="38" t="s">
-        <v>206</v>
+      <c r="A15" s="42"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="54" t="s">
+        <v>205</v>
       </c>
       <c r="L15" t="s">
         <v>186</v>
       </c>
-      <c r="M15" s="39">
+      <c r="M15" s="32">
         <f>2*1024</f>
         <v>2048</v>
       </c>
-      <c r="N15" s="52" t="s">
+      <c r="N15" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="O15" s="52"/>
+      <c r="O15" s="45"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="38"/>
+      <c r="A16" s="42"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="54"/>
       <c r="L16" t="s">
         <v>187</v>
       </c>
@@ -7913,44 +7913,44 @@
         <f>ROUND(M13*M15+M9,0)</f>
         <v>116</v>
       </c>
-      <c r="N16" s="52" t="s">
+      <c r="N16" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="O16" s="52"/>
+      <c r="O16" s="45"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="N17" s="52"/>
-      <c r="O17" s="52"/>
+      <c r="A17" s="42"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="45"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="38" t="s">
-        <v>207</v>
+      <c r="A18" s="42"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="54" t="s">
+        <v>206</v>
       </c>
       <c r="L18" t="s">
         <v>186</v>
       </c>
-      <c r="M18" s="39">
+      <c r="M18" s="32">
         <v>1024</v>
       </c>
-      <c r="N18" s="52" t="s">
+      <c r="N18" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="O18" s="52"/>
+      <c r="O18" s="45"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="44"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="38"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="37"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="54"/>
       <c r="L19" t="s">
         <v>187</v>
       </c>
@@ -7958,43 +7958,43 @@
         <f>ROUND(M13*M18+(M9/2),0)</f>
         <v>58</v>
       </c>
-      <c r="N19" s="52" t="s">
+      <c r="N19" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="O19" s="52"/>
+      <c r="O19" s="45"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="52"/>
-      <c r="O20" s="52"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="45"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="52"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>